<commit_message>
change offer to season at all project
</commit_message>
<xml_diff>
--- a/storage/app/public/reports/unsold_Products.xlsx
+++ b/storage/app/public/reports/unsold_Products.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
   <si>
     <t>ID</t>
   </si>
@@ -39,72 +39,6 @@
   </si>
   <si>
     <t>average rating</t>
-  </si>
-  <si>
-    <t>iPhone 14 Pro</t>
-  </si>
-  <si>
-    <t>A powerful device to keep you connected and entertained on the go. Features a high-resolution camera, fast processor, and long battery life.</t>
-  </si>
-  <si>
-    <t>Smartphones</t>
-  </si>
-  <si>
-    <t>Electronics</t>
-  </si>
-  <si>
-    <t>Wall Art</t>
-  </si>
-  <si>
-    <t>Add a touch of elegance to your space with this wall art.</t>
-  </si>
-  <si>
-    <t>Decor</t>
-  </si>
-  <si>
-    <t>Home</t>
-  </si>
-  <si>
-    <t>Men's Suit</t>
-  </si>
-  <si>
-    <t>Look sharp in this stylish men's suit.</t>
-  </si>
-  <si>
-    <t>Men's Clothing</t>
-  </si>
-  <si>
-    <t>Fashion</t>
-  </si>
-  <si>
-    <t>Nail Polish Set</t>
-  </si>
-  <si>
-    <t>Make your nails look stunning with this nail polish set.</t>
-  </si>
-  <si>
-    <t>Nail Care</t>
-  </si>
-  <si>
-    <t>Sports</t>
-  </si>
-  <si>
-    <t>Treadmill</t>
-  </si>
-  <si>
-    <t>Stay active with this reliable treadmill.</t>
-  </si>
-  <si>
-    <t>Fitness Equipment</t>
-  </si>
-  <si>
-    <t>Soccer Ball</t>
-  </si>
-  <si>
-    <t>Play like a pro with this high-quality soccer ball.</t>
-  </si>
-  <si>
-    <t>Team Sports Gear</t>
   </si>
 </sst>
 </file>
@@ -444,7 +378,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,162 +410,6 @@
       </c>
       <c r="H1" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2">
-        <v>299.99</v>
-      </c>
-      <c r="E2">
-        <v>22</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2">
-        <v>3.75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3">
-        <v>199.99</v>
-      </c>
-      <c r="E3">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4">
-        <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4">
-        <v>299.99</v>
-      </c>
-      <c r="E4">
-        <v>5</v>
-      </c>
-      <c r="F4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5">
-        <v>30</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5">
-        <v>14.99</v>
-      </c>
-      <c r="E5">
-        <v>50</v>
-      </c>
-      <c r="F5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6">
-        <v>31</v>
-      </c>
-      <c r="B6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6">
-        <v>999.99</v>
-      </c>
-      <c r="E6">
-        <v>10</v>
-      </c>
-      <c r="F6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7">
-        <v>33</v>
-      </c>
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7">
-        <v>29.99</v>
-      </c>
-      <c r="E7">
-        <v>50</v>
-      </c>
-      <c r="F7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7">
-        <v>3.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>